<commit_message>
new models are added.
</commit_message>
<xml_diff>
--- a/Evaluations/Blended Skill Talk-COT-results.xlsx
+++ b/Evaluations/Blended Skill Talk-COT-results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1287,6 +1287,128 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Gemma-7B-Instruct</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0.77 ± 0.42</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>-0.03 ± 0.65</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.35 ± 0.71</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.01 ± 0.01</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0.12 ± 0.08</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.01 ± 0.03</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0.11 ± 0.07</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.12 ± 0.09</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0.78 ± 0.23</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0.79 ± 0.23</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0.79 ± 0.23</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0.8 ± 0.24</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0.91 ± 0.27</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0.08 ± 0.12</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>0.46 ± 0.19</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>7.47 ± 1.25</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>0.078 ± 0.00</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>0.87 ± 0.26</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>0.91 ± 0.28</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>2.91 ± 1.36</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>0.47 ± 0.45</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>0.87 ± 0.26</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>1.2 ± 0.42</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Gemini 1.5 Pro is added.
</commit_message>
<xml_diff>
--- a/Evaluations/Blended Skill Talk-COT-results.xlsx
+++ b/Evaluations/Blended Skill Talk-COT-results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1409,6 +1409,100 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>-0.1 ± 0.55</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.44 ± 0.79</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.82 ± 0.1</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.85 ± 0.11</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.84 ± 0.11</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0.9 ± 0.12</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>0.98 ± 0.12</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>0.48 ± 0.14</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>5.21 ± 5.4</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>0.015 ± 0.00</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>0.92 ± 0.12</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>0.97 ± 0.15</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>2.96 ± 1.27</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>0.54 ± 0.41</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>0.92 ± 0.12</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>1.26 ± 0.31</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>